<commit_message>
Regex para extraer el nombre, habitación, arr_date y dep_date del room report  añadido
</commit_message>
<xml_diff>
--- a/daily_excel.xlsx
+++ b/daily_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\WorkScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48BD9C8-418A-4F45-8099-511291B9A041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11208AE3-31D4-497F-81F1-83DA1AEA6854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8550" yWindow="2730" windowWidth="29040" windowHeight="15720" xr2:uid="{24227F4B-AA81-4BA6-A47D-2A7D1043BB9B}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24227F4B-AA81-4BA6-A47D-2A7D1043BB9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -482,6 +482,51 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -491,15 +536,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -507,42 +543,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -880,440 +880,439 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59984A97-E6A4-4094-B6EC-5EA7E51BA644}">
-  <dimension ref="B3:R42"/>
+  <dimension ref="A3:Q42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="3:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="28" t="s">
+    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
-      <c r="G4" s="31" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="F4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="33"/>
-    </row>
-    <row r="5" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="3:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="22" t="s">
+    </row>
+    <row r="6" spans="2:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="G6" s="22" t="s">
+      <c r="C6" s="20"/>
+      <c r="D6" s="21"/>
+      <c r="F6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="34"/>
-    </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-    </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
-      <c r="M13" s="7"/>
-    </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
-      <c r="R14" s="7"/>
-    </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="12"/>
-      <c r="K18" s="7"/>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="12"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="12"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="12"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="12"/>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="12"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="12"/>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="10"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="12"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="12"/>
-      <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="10"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="12"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="15"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="15"/>
-    </row>
-    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="16"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="3" t="s">
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="34"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="12"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="12"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="10"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="12"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="12"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="10"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="12"/>
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="12"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="12"/>
+    </row>
+    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="28"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="30"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="18"/>
-    </row>
-    <row r="35" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="10"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="8" t="s">
+      <c r="F34" s="25"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="27"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G35" s="10"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="10"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="2" t="s">
+      <c r="F35" s="10"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="10"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="6"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="9" t="s">
+      <c r="F36" s="10"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="12"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="10"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="10"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="9" t="s">
+      <c r="F37" s="10"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="12"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="10"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G38" s="10"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="12"/>
-    </row>
-    <row r="39" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="10"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="9" t="s">
+      <c r="F38" s="10"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="12"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="10"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="10"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="12"/>
-    </row>
-    <row r="40" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="10"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="9" t="s">
+      <c r="F39" s="10"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="12"/>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="10"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="10"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="12"/>
-    </row>
-    <row r="41" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="19"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="2" t="s">
+      <c r="F40" s="10"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="12"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="13"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="15"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F41" s="28"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="30"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="F41:H41"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>